<commit_message>
sn: update ia 2024
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Senegal/2024/oct 2024/sn_sch_sth_impact_202410_1_site.xlsx
+++ b/SCH-STH/Impact assessments/Senegal/2024/oct 2024/sn_sch_sth_impact_202410_1_site.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Senegal\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Senegal\2024\oct 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7507F548-B674-432C-93EF-23D2F3D7AD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40CFE92-A5E9-4E66-9B40-CC028FBB20F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="498" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="498" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2964,12 +2964,6 @@
     <t>(${w_source_exist_school} = 'Oui' or ${w_source_exist_village} = 'Oui') and (${w_consent_village} = 'Oui' or ${w_consent_school} = 'Oui')</t>
   </si>
   <si>
-    <t>(2024 Mar) - 1. SCH/STH – Site V4</t>
-  </si>
-  <si>
-    <t>sn_sch_sth_impact_202403_1_site_v4</t>
-  </si>
-  <si>
     <t>6.1. Le site est-il une école ou un mileiu communautaire?</t>
   </si>
   <si>
@@ -3091,6 +3085,12 @@
   </si>
   <si>
     <t>EE TENDINE</t>
+  </si>
+  <si>
+    <t>sn_sch_sth_impact_202410_1_site</t>
+  </si>
+  <si>
+    <t>(2024 Oct) - 1. SCH/STH – Site</t>
   </si>
 </sst>
 </file>
@@ -3631,147 +3631,7 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{5BE5DCD7-EA3A-4378-8DB1-F4C861BED5B4}"/>
     <cellStyle name="Normal 3 2" xfId="2" xr:uid="{057D505D-6799-463F-A486-074478D809DD}"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4183,8 +4043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
@@ -4426,7 +4286,7 @@
         <v>876</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="18"/>
@@ -4713,10 +4573,10 @@
         <v>24</v>
       </c>
       <c r="B21" s="64" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="18"/>
@@ -4739,7 +4599,7 @@
         <v>842</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="18"/>
@@ -4762,7 +4622,7 @@
         <v>843</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="18"/>
@@ -4785,7 +4645,7 @@
         <v>844</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="18"/>
@@ -4808,7 +4668,7 @@
         <v>845</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D25" s="73"/>
       <c r="E25" s="25"/>
@@ -4831,7 +4691,7 @@
         <v>846</v>
       </c>
       <c r="C26" s="72" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D26" s="73"/>
       <c r="E26" s="25"/>
@@ -4854,7 +4714,7 @@
         <v>847</v>
       </c>
       <c r="C27" s="72" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D27" s="73"/>
       <c r="E27" s="25"/>
@@ -4877,7 +4737,7 @@
         <v>848</v>
       </c>
       <c r="C28" s="72" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D28" s="73"/>
       <c r="E28" s="25"/>
@@ -4907,7 +4767,7 @@
       <c r="F29" s="25"/>
       <c r="G29" s="73"/>
       <c r="H29" s="21" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="I29" s="25"/>
       <c r="J29" s="18" t="s">
@@ -4945,10 +4805,10 @@
         <v>24</v>
       </c>
       <c r="B31" s="64" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C31" s="72" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D31" s="73"/>
       <c r="E31" s="25"/>
@@ -4973,14 +4833,14 @@
         <v>135</v>
       </c>
       <c r="C32" s="72" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D32" s="73"/>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
       <c r="G32" s="73"/>
       <c r="H32" s="21" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="18" t="s">
@@ -4998,14 +4858,14 @@
         <v>136</v>
       </c>
       <c r="C33" s="72" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D33" s="73"/>
       <c r="E33" s="25"/>
       <c r="F33" s="25"/>
       <c r="G33" s="73"/>
       <c r="H33" s="21" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="I33" s="25"/>
       <c r="J33" s="18" t="s">
@@ -5023,7 +4883,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>23</v>
@@ -5073,7 +4933,7 @@
         <v>28</v>
       </c>
       <c r="C36" s="72" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="D36" s="73"/>
       <c r="E36" s="25"/>
@@ -5155,9 +5015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6459,10 +6319,10 @@
         <v>35</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C114" s="25" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D114" s="20" t="s">
         <v>271</v>
@@ -6669,10 +6529,10 @@
         <v>35</v>
       </c>
       <c r="B129" s="25" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C129" s="25" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D129" s="20" t="s">
         <v>271</v>
@@ -9515,10 +9375,10 @@
         <v>75</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E333" t="s">
         <v>274</v>
@@ -9529,10 +9389,10 @@
         <v>75</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C334" s="4" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E334" t="s">
         <v>274</v>
@@ -9543,10 +9403,10 @@
         <v>75</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C335" s="4" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E335" t="s">
         <v>311</v>
@@ -9599,10 +9459,10 @@
         <v>75</v>
       </c>
       <c r="B339" s="4" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E339" t="s">
         <v>291</v>
@@ -10481,10 +10341,10 @@
         <v>75</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E402" t="s">
         <v>293</v>
@@ -10831,10 +10691,10 @@
         <v>75</v>
       </c>
       <c r="B427" s="4" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E427" t="s">
         <v>287</v>
@@ -10845,10 +10705,10 @@
         <v>75</v>
       </c>
       <c r="B428" s="4" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E428" t="s">
         <v>287</v>
@@ -11293,10 +11153,10 @@
         <v>75</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C460" s="4" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E460" t="s">
         <v>289</v>
@@ -11629,10 +11489,10 @@
         <v>75</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="E484" t="s">
         <v>314</v>
@@ -11643,10 +11503,10 @@
         <v>75</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E485" t="s">
         <v>275</v>
@@ -11923,13 +11783,13 @@
         <v>75</v>
       </c>
       <c r="B505" s="4" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C505" s="4" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E505" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
@@ -11943,7 +11803,7 @@
         <v>684</v>
       </c>
       <c r="E506" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
@@ -12315,10 +12175,10 @@
         <v>75</v>
       </c>
       <c r="B533" s="4" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C533" s="4" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="E533" t="s">
         <v>303</v>
@@ -12343,10 +12203,10 @@
         <v>75</v>
       </c>
       <c r="B535" s="4" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C535" s="4" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E535" t="s">
         <v>294</v>
@@ -12357,10 +12217,10 @@
         <v>75</v>
       </c>
       <c r="B536" s="4" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="E536" t="s">
         <v>294</v>
@@ -15325,10 +15185,10 @@
         <v>75</v>
       </c>
       <c r="B748" s="4" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C748" s="4" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E748" t="s">
         <v>288</v>
@@ -15451,10 +15311,10 @@
         <v>75</v>
       </c>
       <c r="B757" s="4" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C757" s="4" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="E757" t="s">
         <v>306</v>
@@ -15493,10 +15353,10 @@
         <v>75</v>
       </c>
       <c r="B760" s="4" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C760" s="4" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E760" t="s">
         <v>316</v>
@@ -15619,10 +15479,10 @@
         <v>75</v>
       </c>
       <c r="B769" s="4" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C769" s="4" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E769" t="s">
         <v>619</v>
@@ -15633,10 +15493,10 @@
         <v>75</v>
       </c>
       <c r="B770" s="4" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C770" s="4" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E770" t="s">
         <v>619</v>
@@ -15647,10 +15507,10 @@
         <v>75</v>
       </c>
       <c r="B771" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C771" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E771" t="s">
         <v>317</v>
@@ -15689,10 +15549,10 @@
         <v>75</v>
       </c>
       <c r="B774" s="4" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C774" s="4" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="E774" t="s">
         <v>616</v>
@@ -15709,7 +15569,7 @@
         <v>710</v>
       </c>
       <c r="E775" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="776" spans="1:5" x14ac:dyDescent="0.25">
@@ -15723,7 +15583,7 @@
         <v>709</v>
       </c>
       <c r="E776" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="777" spans="1:5" x14ac:dyDescent="0.25">
@@ -17650,7 +17510,7 @@
         <v>213</v>
       </c>
       <c r="F910" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="911" spans="1:6" x14ac:dyDescent="0.25">
@@ -17664,7 +17524,7 @@
         <v>214</v>
       </c>
       <c r="F911" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="912" spans="1:6" x14ac:dyDescent="0.25">
@@ -17678,7 +17538,7 @@
         <v>215</v>
       </c>
       <c r="F912" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="913" spans="1:6" x14ac:dyDescent="0.25">
@@ -17734,7 +17594,7 @@
         <v>219</v>
       </c>
       <c r="F916" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="917" spans="1:6" x14ac:dyDescent="0.25">
@@ -17916,7 +17776,7 @@
         <v>232</v>
       </c>
       <c r="F929" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="930" spans="1:6" x14ac:dyDescent="0.25">
@@ -18042,7 +17902,7 @@
         <v>241</v>
       </c>
       <c r="F938" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="939" spans="1:6" x14ac:dyDescent="0.25">
@@ -18056,7 +17916,7 @@
         <v>242</v>
       </c>
       <c r="F939" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="940" spans="1:6" x14ac:dyDescent="0.25">
@@ -18084,7 +17944,7 @@
         <v>244</v>
       </c>
       <c r="F941" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="942" spans="1:6" x14ac:dyDescent="0.25">
@@ -18140,7 +18000,7 @@
         <v>248</v>
       </c>
       <c r="F945" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="946" spans="1:6" x14ac:dyDescent="0.25">
@@ -18154,7 +18014,7 @@
         <v>249</v>
       </c>
       <c r="F946" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="947" spans="1:6" x14ac:dyDescent="0.25">
@@ -18182,7 +18042,7 @@
         <v>251</v>
       </c>
       <c r="F948" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="949" spans="1:6" x14ac:dyDescent="0.25">
@@ -18238,7 +18098,7 @@
         <v>255</v>
       </c>
       <c r="F952" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="953" spans="1:6" x14ac:dyDescent="0.25">
@@ -18266,7 +18126,7 @@
         <v>257</v>
       </c>
       <c r="F954" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="955" spans="1:6" x14ac:dyDescent="0.25">
@@ -18280,7 +18140,7 @@
         <v>258</v>
       </c>
       <c r="F955" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="956" spans="1:6" x14ac:dyDescent="0.25">
@@ -18420,7 +18280,7 @@
         <v>268</v>
       </c>
       <c r="F965" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="966" spans="1:6" x14ac:dyDescent="0.25">
@@ -18434,7 +18294,7 @@
         <v>269</v>
       </c>
       <c r="F966" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="967" spans="1:6" x14ac:dyDescent="0.25">
@@ -18476,7 +18336,7 @@
         <v>272</v>
       </c>
       <c r="F969" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="970" spans="1:6" x14ac:dyDescent="0.25">
@@ -18518,7 +18378,7 @@
         <v>275</v>
       </c>
       <c r="F972" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="973" spans="1:6" x14ac:dyDescent="0.25">
@@ -18532,7 +18392,7 @@
         <v>276</v>
       </c>
       <c r="F973" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="974" spans="1:6" x14ac:dyDescent="0.25">
@@ -18546,7 +18406,7 @@
         <v>277</v>
       </c>
       <c r="F974" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="975" spans="1:6" x14ac:dyDescent="0.25">
@@ -18588,7 +18448,7 @@
         <v>280</v>
       </c>
       <c r="F977" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="978" spans="1:6" x14ac:dyDescent="0.25">
@@ -22635,7 +22495,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -22658,10 +22518,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>907</v>
+        <v>949</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>908</v>
+        <v>948</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -22678,7 +22538,7 @@
   <dimension ref="A1:V469"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A421" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2:D469"/>
     </sheetView>
   </sheetViews>
@@ -22974,7 +22834,7 @@
         <v>274</v>
       </c>
       <c r="V6" s="53" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -23021,7 +22881,7 @@
         <v>274</v>
       </c>
       <c r="V7" s="53" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -23068,7 +22928,7 @@
         <v>311</v>
       </c>
       <c r="V8" s="53" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -23244,7 +23104,7 @@
         <v>291</v>
       </c>
       <c r="V12" s="53" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -23648,7 +23508,7 @@
         <v>271</v>
       </c>
       <c r="S22" s="53" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="U22" s="53" t="s">
         <v>576</v>
@@ -24263,7 +24123,7 @@
         <v>271</v>
       </c>
       <c r="S37" s="57" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="U37" s="57" t="s">
         <v>302</v>
@@ -25827,7 +25687,7 @@
         <v>293</v>
       </c>
       <c r="V75" s="53" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
@@ -26852,7 +26712,7 @@
         <v>287</v>
       </c>
       <c r="V100" s="53" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.25">
@@ -26893,7 +26753,7 @@
         <v>287</v>
       </c>
       <c r="V101" s="53" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.25">
@@ -27399,7 +27259,7 @@
         <v>274</v>
       </c>
       <c r="D114" s="53" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E114">
         <v>213</v>
@@ -27440,7 +27300,7 @@
         <v>274</v>
       </c>
       <c r="D115" s="53" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E115">
         <v>214</v>
@@ -27481,7 +27341,7 @@
         <v>311</v>
       </c>
       <c r="D116" s="53" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E116">
         <v>215</v>
@@ -27645,7 +27505,7 @@
         <v>291</v>
       </c>
       <c r="D120" s="53" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E120">
         <v>219</v>
@@ -28178,7 +28038,7 @@
         <v>293</v>
       </c>
       <c r="D133" s="53" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E133">
         <v>232</v>
@@ -28205,7 +28065,7 @@
         <v>289</v>
       </c>
       <c r="V133" s="53" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="134" spans="1:22" x14ac:dyDescent="0.25">
@@ -28547,7 +28407,7 @@
         <v>287</v>
       </c>
       <c r="D142" s="53" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E142">
         <v>241</v>
@@ -28588,7 +28448,7 @@
         <v>287</v>
       </c>
       <c r="D143" s="53" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E143">
         <v>242</v>
@@ -28670,7 +28530,7 @@
         <v>289</v>
       </c>
       <c r="D145" s="53" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E145">
         <v>244</v>
@@ -28834,7 +28694,7 @@
         <v>314</v>
       </c>
       <c r="D149" s="53" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="E149">
         <v>248</v>
@@ -28875,7 +28735,7 @@
         <v>275</v>
       </c>
       <c r="D150" s="53" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E150">
         <v>249</v>
@@ -28954,10 +28814,10 @@
         <v>271</v>
       </c>
       <c r="C152" s="53" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D152" s="53" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E152">
         <v>251</v>
@@ -28995,7 +28855,7 @@
         <v>271</v>
       </c>
       <c r="C153" s="53" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D153" s="53" t="s">
         <v>684</v>
@@ -29121,7 +28981,7 @@
         <v>303</v>
       </c>
       <c r="D156" s="53" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="E156">
         <v>255</v>
@@ -29189,7 +29049,7 @@
         <v>314</v>
       </c>
       <c r="V157" s="53" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="158" spans="1:22" x14ac:dyDescent="0.25">
@@ -29203,7 +29063,7 @@
         <v>294</v>
       </c>
       <c r="D158" s="53" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E158">
         <v>257</v>
@@ -29230,7 +29090,7 @@
         <v>275</v>
       </c>
       <c r="V158" s="53" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="159" spans="1:22" x14ac:dyDescent="0.25">
@@ -29244,7 +29104,7 @@
         <v>294</v>
       </c>
       <c r="D159" s="53" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="E159">
         <v>258</v>
@@ -29654,7 +29514,7 @@
         <v>288</v>
       </c>
       <c r="D169" s="53" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E169">
         <v>268</v>
@@ -29695,7 +29555,7 @@
         <v>306</v>
       </c>
       <c r="D170" s="53" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="E170">
         <v>269</v>
@@ -29818,7 +29678,7 @@
         <v>316</v>
       </c>
       <c r="D173" s="53" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E173">
         <v>272</v>
@@ -29941,7 +29801,7 @@
         <v>619</v>
       </c>
       <c r="D176" s="53" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E176">
         <v>275</v>
@@ -29982,7 +29842,7 @@
         <v>619</v>
       </c>
       <c r="D177" s="53" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E177">
         <v>276</v>
@@ -30023,7 +29883,7 @@
         <v>317</v>
       </c>
       <c r="D178" s="53" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E178">
         <v>277</v>
@@ -30047,10 +29907,10 @@
         <v>459</v>
       </c>
       <c r="U178" s="53" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="V178" s="53" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.25">
@@ -30088,7 +29948,7 @@
         <v>462</v>
       </c>
       <c r="U179" s="53" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="V179" s="53" t="s">
         <v>684</v>
@@ -30146,7 +30006,7 @@
         <v>616</v>
       </c>
       <c r="D181" s="53" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="E181">
         <v>280</v>
@@ -30184,7 +30044,7 @@
         <v>271</v>
       </c>
       <c r="C182" s="53" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D182" s="53" t="s">
         <v>710</v>
@@ -30225,7 +30085,7 @@
         <v>271</v>
       </c>
       <c r="C183" s="53" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D183" s="53" t="s">
         <v>709</v>
@@ -31198,7 +31058,7 @@
         <v>303</v>
       </c>
       <c r="V206" s="53" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="207" spans="1:22" x14ac:dyDescent="0.25">
@@ -31280,7 +31140,7 @@
         <v>294</v>
       </c>
       <c r="V208" s="53" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="209" spans="1:22" x14ac:dyDescent="0.25">
@@ -31321,7 +31181,7 @@
         <v>294</v>
       </c>
       <c r="V209" s="53" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="210" spans="1:22" x14ac:dyDescent="0.25">
@@ -37781,7 +37641,7 @@
         <v>288</v>
       </c>
       <c r="V421" s="53" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="422" spans="1:22" x14ac:dyDescent="0.25">
@@ -38042,7 +37902,7 @@
         <v>306</v>
       </c>
       <c r="V430" s="53" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="431" spans="1:22" x14ac:dyDescent="0.25">
@@ -38129,7 +37989,7 @@
         <v>316</v>
       </c>
       <c r="V433" s="53" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="434" spans="1:22" x14ac:dyDescent="0.25">
@@ -38390,7 +38250,7 @@
         <v>619</v>
       </c>
       <c r="V442" s="53" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="443" spans="1:22" x14ac:dyDescent="0.25">
@@ -38419,7 +38279,7 @@
         <v>619</v>
       </c>
       <c r="V443" s="53" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="444" spans="1:22" x14ac:dyDescent="0.25">
@@ -38448,7 +38308,7 @@
         <v>317</v>
       </c>
       <c r="V444" s="53" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="445" spans="1:22" x14ac:dyDescent="0.25">
@@ -38535,7 +38395,7 @@
         <v>616</v>
       </c>
       <c r="V447" s="53" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="448" spans="1:22" x14ac:dyDescent="0.25">
@@ -38561,7 +38421,7 @@
         <v>710</v>
       </c>
       <c r="U448" s="53" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="V448" s="53" t="s">
         <v>710</v>
@@ -38590,7 +38450,7 @@
         <v>709</v>
       </c>
       <c r="U449" s="53" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="V449" s="53" t="s">
         <v>709</v>

</xml_diff>